<commit_message>
mais dados ciclo-2 e arrumada no relatorio
</commit_message>
<xml_diff>
--- a/atvmans.xlsx
+++ b/atvmans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Desktop\Task manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D251ECB-16F7-4C11-99C8-5B54AC1D8BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AAB50D-3EBE-4BDD-B1C8-1B8ED5E25D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15090" yWindow="1950" windowWidth="18420" windowHeight="12135" xr2:uid="{FD453EF9-81AA-49AE-A837-A80D398E3442}"/>
+    <workbookView xWindow="5295" yWindow="2070" windowWidth="18420" windowHeight="12135" xr2:uid="{FD453EF9-81AA-49AE-A837-A80D398E3442}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,15 +650,15 @@
         <v>2</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" ref="E6:E15" si="3">C7</f>
-        <v>0.68600000000000017</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C7-E7</f>
+        <v>0.68600000000000017</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -677,15 +677,14 @@
         <v>2</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="3"/>
-        <v>0.58799999999999997</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.58799999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -704,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E7:E14" si="3">C9</f>
         <v>0.58799999999999997</v>
       </c>
       <c r="F9" t="s">

</xml_diff>